<commit_message>
add metro map plan flag
</commit_message>
<xml_diff>
--- a/doc/data.xlsx
+++ b/doc/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="556">
   <si>
     <t>bj</t>
   </si>
@@ -4561,6 +4561,10 @@
       </rPr>
       <t>济南</t>
     </r>
+  </si>
+  <si>
+    <t>Plan</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -4948,9 +4952,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K37" sqref="K2:K37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4965,7 +4971,7 @@
     <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>100</v>
       </c>
@@ -4990,11 +4996,14 @@
       <c r="H1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -5017,12 +5026,15 @@
         <v>107</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="J2" s="2" t="str">
-        <f>"{ " &amp; LOWER($A$1) &amp; ": """ &amp; A2 &amp; """, " &amp; LOWER($B$1) &amp; ": " &amp; B2 &amp; ", " &amp; LOWER($C$1) &amp; ": " &amp; C2 &amp; ", " &amp; LOWER($D$1) &amp; ": """ &amp; D2 &amp; """, " &amp; LOWER($E$1) &amp; ": """ &amp; E2 &amp; """, " &amp; LOWER($F$1) &amp; ": """ &amp; F2 &amp; """, " &amp; LOWER($G$1) &amp; ": """ &amp; G2 &amp; """, " &amp; LOWER($H$1) &amp; ": """ &amp; H2 &amp; """" &amp;  " },"</f>
-        <v>{ key: "bj", lat: 39.908065, lng: 116.411502, name: "北京", english: "Beijing", pinyin: "beijing", py: "bj", other: "" },</v>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="str">
+        <f>"{ " &amp; LOWER($A$1) &amp; ": """ &amp; A2 &amp; """, " &amp; LOWER($B$1) &amp; ": " &amp; B2 &amp; ", " &amp; LOWER($C$1) &amp; ": " &amp; C2 &amp; ", " &amp; LOWER($D$1) &amp; ": """ &amp; D2 &amp; """, " &amp; LOWER($E$1) &amp; ": """ &amp; E2 &amp; """, " &amp; LOWER($F$1) &amp; ": """ &amp; F2 &amp; """, " &amp; LOWER($G$1) &amp; ": """ &amp; G2 &amp; """, " &amp; LOWER($H$1) &amp; ": """ &amp; H2 &amp; """, " &amp; LOWER($I$1) &amp; ": """ &amp; I2 &amp; """" &amp;  " },"</f>
+        <v>{ key: "bj", lat: 39.908065, lng: 116.411502, name: "北京", english: "Beijing", pinyin: "beijing", py: "bj", other: "", plan: "1" },</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -5045,12 +5057,15 @@
         <v>108</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J37" si="0">"{ " &amp; LOWER($A$1) &amp; ": """ &amp; A3 &amp; """, " &amp; LOWER($B$1) &amp; ": " &amp; B3 &amp; ", " &amp; LOWER($C$1) &amp; ": " &amp; C3 &amp; ", " &amp; LOWER($D$1) &amp; ": """ &amp; D3 &amp; """, " &amp; LOWER($E$1) &amp; ": """ &amp; E3 &amp; """, " &amp; LOWER($F$1) &amp; ": """ &amp; F3 &amp; """, " &amp; LOWER($G$1) &amp; ": """ &amp; G3 &amp; """, " &amp; LOWER($H$1) &amp; ": """ &amp; H3 &amp; """" &amp;  " },"</f>
-        <v>{ key: "sh", lat: 31.232844, lng: 121.47537, name: "上海", english: "Shanghai", pinyin: "shanghai", py: "sh", other: "" },</v>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="str">
+        <f t="shared" ref="K3:K37" si="0">"{ " &amp; LOWER($A$1) &amp; ": """ &amp; A3 &amp; """, " &amp; LOWER($B$1) &amp; ": " &amp; B3 &amp; ", " &amp; LOWER($C$1) &amp; ": " &amp; C3 &amp; ", " &amp; LOWER($D$1) &amp; ": """ &amp; D3 &amp; """, " &amp; LOWER($E$1) &amp; ": """ &amp; E3 &amp; """, " &amp; LOWER($F$1) &amp; ": """ &amp; F3 &amp; """, " &amp; LOWER($G$1) &amp; ": """ &amp; G3 &amp; """, " &amp; LOWER($H$1) &amp; ": """ &amp; H3 &amp; """, " &amp; LOWER($I$1) &amp; ": """ &amp; I3 &amp; """" &amp;  " },"</f>
+        <v>{ key: "sh", lat: 31.232844, lng: 121.47537, name: "上海", english: "Shanghai", pinyin: "shanghai", py: "sh", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -5075,12 +5090,15 @@
       <c r="H4" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="J4" s="2" t="str">
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "gz", lat: 23.111459, lng: 113.324103, name: "广州(佛山)", english: "Guangzhou", pinyin: "guangzhou", py: "gz", other: "foshan|fs" },</v>
+        <v>{ key: "gz", lat: 23.111459, lng: 113.324103, name: "广州(佛山)", english: "Guangzhou", pinyin: "guangzhou", py: "gz", other: "foshan|fs", plan: "0" },</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -5103,12 +5121,15 @@
         <v>110</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="J5" s="2" t="str">
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "sz", lat: 22.541455, lng: 114.052827, name: "深圳", english: "Shenzhen", pinyin: "shenzhen", py: "sz", other: "" },</v>
+        <v>{ key: "sz", lat: 22.541455, lng: 114.052827, name: "深圳", english: "Shenzhen", pinyin: "shenzhen", py: "sz", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -5133,12 +5154,15 @@
       <c r="H6" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="J6" s="2" t="str">
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "hk", lat: 22.284659, lng: 114.158185, name: "香港", english: "Hong Kong", pinyin: "xianggang", py: "xg", other: "hk|hongkong|hong kong" },</v>
+        <v>{ key: "hk", lat: 22.284659, lng: 114.158185, name: "香港", english: "Hong Kong", pinyin: "xianggang", py: "xg", other: "hk|hongkong|hong kong", plan: "0" },</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -5163,12 +5187,15 @@
       <c r="H7" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="J7" s="2" t="str">
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "tb", lat: 25.046256, lng: 121.51753, name: "台北", english: "Taipei", pinyin: "taibei", py: "tb", other: "tp|taipei" },</v>
+        <v>{ key: "tb", lat: 25.046256, lng: 121.51753, name: "台北", english: "Taipei", pinyin: "taibei", py: "tb", other: "tp|taipei", plan: "0" },</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -5191,12 +5218,15 @@
         <v>115</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="J8" s="2" t="str">
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "nj", lat: 32.040995, lng: 118.78408, name: "南京", english: "Nanjing", pinyin: "nanjing", py: "nj", other: "" },</v>
+        <v>{ key: "nj", lat: 32.040995, lng: 118.78408, name: "南京", english: "Nanjing", pinyin: "nanjing", py: "nj", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -5219,12 +5249,15 @@
         <v>116</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="J9" s="2" t="str">
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "tj", lat: 39.137775, lng: 117.21161, name: "天津", english: "Tianjin", pinyin: "tianjin", py: "tj", other: "" },</v>
+        <v>{ key: "tj", lat: 39.137775, lng: 117.21161, name: "天津", english: "Tianjin", pinyin: "tianjin", py: "tj", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
@@ -5247,12 +5280,15 @@
         <v>117</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="J10" s="2" t="str">
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "cq", lat: 29.552992, lng: 106.548273, name: "重庆", english: "Chongqing", pinyin: "chongqing", py: "cq", other: "" },</v>
+        <v>{ key: "cq", lat: 29.552992, lng: 106.548273, name: "重庆", english: "Chongqing", pinyin: "chongqing", py: "cq", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -5275,12 +5311,15 @@
         <v>118</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="J11" s="2" t="str">
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "cd", lat: 30.658071, lng: 104.065798, name: "成都", english: "Chengdu", pinyin: "chengdu", py: "cd", other: "" },</v>
+        <v>{ key: "cd", lat: 30.658071, lng: 104.065798, name: "成都", english: "Chengdu", pinyin: "chengdu", py: "cd", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -5303,12 +5342,15 @@
         <v>119</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="J12" s="2" t="str">
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "wh", lat: 30.585299, lng: 114.286584, name: "武汉", english: "Wuhan", pinyin: "wuhan", py: "wh", other: "" },</v>
+        <v>{ key: "wh", lat: 30.585299, lng: 114.286584, name: "武汉", english: "Wuhan", pinyin: "wuhan", py: "wh", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
@@ -5331,12 +5373,15 @@
         <v>120</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="J13" s="2" t="str">
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "hz", lat: 30.279156, lng: 120.165666, name: "杭州", english: "Hangzhou", pinyin: "hangzhou", py: "hz", other: "" },</v>
+        <v>{ key: "hz", lat: 30.279156, lng: 120.165666, name: "杭州", english: "Hangzhou", pinyin: "hangzhou", py: "hz", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
@@ -5359,12 +5404,15 @@
         <v>121</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="J14" s="2" t="str">
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "xa", lat: 34.269878, lng: 108.947143, name: "西安", english: "Xi'an", pinyin: "xian", py: "xa", other: "" },</v>
+        <v>{ key: "xa", lat: 34.269878, lng: 108.947143, name: "西安", english: "Xi'an", pinyin: "xian", py: "xa", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -5387,12 +5435,15 @@
         <v>110</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="J15" s="2" t="str">
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "su", lat: 31.29273, lng: 120.549292, name: "苏州", english: "Suzhou", pinyin: "suzhou", py: "sz", other: "" },</v>
+        <v>{ key: "su", lat: 31.29273, lng: 120.549292, name: "苏州", english: "Suzhou", pinyin: "suzhou", py: "sz", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
@@ -5415,12 +5466,15 @@
         <v>123</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="J16" s="2" t="str">
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "sy", lat: 41.792353, lng: 123.433386, name: "沈阳", english: "Shenyang", pinyin: "shenyang", py: "sy", other: "" },</v>
+        <v>{ key: "sy", lat: 41.792353, lng: 123.433386, name: "沈阳", english: "Shenyang", pinyin: "shenyang", py: "sy", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -5443,12 +5497,15 @@
         <v>124</v>
       </c>
       <c r="H17" s="1"/>
-      <c r="J17" s="2" t="str">
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "cc", lat: 43.833106, lng: 125.365183, name: "长春", english: "Changchun", pinyin: "changchun", py: "cc", other: "" },</v>
+        <v>{ key: "cc", lat: 43.833106, lng: 125.365183, name: "长春", english: "Changchun", pinyin: "changchun", py: "cc", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
@@ -5471,12 +5528,15 @@
         <v>125</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="J18" s="2" t="str">
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "hb", lat: 45.75837, lng: 126.643805, name: "哈尔滨", english: "Harbin", pinyin: "harbin", py: "hrb", other: "" },</v>
+        <v>{ key: "hb", lat: 45.75837, lng: 126.643805, name: "哈尔滨", english: "Harbin", pinyin: "harbin", py: "hrb", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -5499,12 +5559,15 @@
         <v>126</v>
       </c>
       <c r="H19" s="1"/>
-      <c r="J19" s="2" t="str">
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "cs", lat: 28.195185, lng: 112.976357, name: "长沙", english: "Changsha", pinyin: "changsha", py: "cs", other: "" },</v>
+        <v>{ key: "cs", lat: 28.195185, lng: 112.976357, name: "长沙", english: "Changsha", pinyin: "changsha", py: "cs", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
@@ -5527,12 +5590,15 @@
         <v>127</v>
       </c>
       <c r="H20" s="1"/>
-      <c r="J20" s="2" t="str">
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "nb", lat: 29.873025, lng: 121.548731, name: "宁波", english: "Ningbo", pinyin: "ningbo", py: "nb", other: "" },</v>
+        <v>{ key: "nb", lat: 29.873025, lng: 121.548731, name: "宁波", english: "Ningbo", pinyin: "ningbo", py: "nb", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
@@ -5555,12 +5621,15 @@
         <v>128</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="J21" s="2" t="str">
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "wx", lat: 31.589211, lng: 120.306895, name: "无锡", english: "Wuxi", pinyin: "wuxi", py: "wx", other: "" },</v>
+        <v>{ key: "wx", lat: 31.589211, lng: 120.306895, name: "无锡", english: "Wuxi", pinyin: "wuxi", py: "wx", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
@@ -5583,12 +5652,15 @@
         <v>129</v>
       </c>
       <c r="H22" s="1"/>
-      <c r="J22" s="2" t="str">
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "zz", lat: 34.746867, lng: 113.655446, name: "郑州", english: "Zhengzhou", pinyin: "zhengzhou", py: "zz", other: "" },</v>
+        <v>{ key: "zz", lat: 34.746867, lng: 113.655446, name: "郑州", english: "Zhengzhou", pinyin: "zhengzhou", py: "zz", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
@@ -5611,12 +5683,15 @@
         <v>130</v>
       </c>
       <c r="H23" s="1"/>
-      <c r="J23" s="2" t="str">
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "dl", lat: 38.909368, lng: 121.587378, name: "大连", english: "Dalian", pinyin: "dalian", py: "dl", other: "" },</v>
+        <v>{ key: "dl", lat: 38.909368, lng: 121.587378, name: "大连", english: "Dalian", pinyin: "dalian", py: "dl", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>57</v>
       </c>
@@ -5639,12 +5714,15 @@
         <v>131</v>
       </c>
       <c r="H24" s="1"/>
-      <c r="J24" s="2" t="str">
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "km", lat: 25.013618, lng: 102.723847, name: "昆明", english: "Kunming", pinyin: "kunming", py: "km", other: "" },</v>
+        <v>{ key: "km", lat: 25.013618, lng: 102.723847, name: "昆明", english: "Kunming", pinyin: "kunming", py: "km", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
@@ -5667,12 +5745,15 @@
         <v>132</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="J25" s="2" t="str">
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "nc", lat: 28.67542, lng: 115.903436, name: "南昌", english: "Nanchang", pinyin: "nanchang", py: "nc", other: "" },</v>
+        <v>{ key: "nc", lat: 28.67542, lng: 115.903436, name: "南昌", english: "Nanchang", pinyin: "nanchang", py: "nc", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>59</v>
       </c>
@@ -5695,12 +5776,15 @@
         <v>133</v>
       </c>
       <c r="H26" s="1"/>
-      <c r="J26" s="2" t="str">
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "qd", lat: 36.169772, lng: 120.376824, name: "青岛", english: "Qingdao", pinyin: "qingdao", py: "qd", other: "" },</v>
+        <v>{ key: "qd", lat: 36.169772, lng: 120.376824, name: "青岛", english: "Qingdao", pinyin: "qingdao", py: "qd", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>60</v>
       </c>
@@ -5723,12 +5807,15 @@
         <v>134</v>
       </c>
       <c r="H27" s="1"/>
-      <c r="J27" s="2" t="str">
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "dg", lat: 23.089687, lng: 113.860969, name: "东莞", english: "Dongguan", pinyin: "dongguan", py: "dg", other: "" },</v>
+        <v>{ key: "dg", lat: 23.089687, lng: 113.860969, name: "东莞", english: "Dongguan", pinyin: "dongguan", py: "dg", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>61</v>
       </c>
@@ -5751,12 +5838,15 @@
         <v>135</v>
       </c>
       <c r="H28" s="1"/>
-      <c r="J28" s="2" t="str">
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "nn", lat: 22.839824, lng: 108.413459, name: "南宁", english: "Nanning", pinyin: "nanning", py: "nn", other: "" },</v>
+        <v>{ key: "nn", lat: 22.839824, lng: 108.413459, name: "南宁", english: "Nanning", pinyin: "nanning", py: "nn", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
@@ -5779,12 +5869,15 @@
         <v>136</v>
       </c>
       <c r="H29" s="1"/>
-      <c r="J29" s="2" t="str">
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "fz", lat: 25.985736, lng: 119.39006, name: "福州", english: "Fuzhou", pinyin: "fuzhou", py: "fz", other: "" },</v>
+        <v>{ key: "fz", lat: 25.985736, lng: 119.39006, name: "福州", english: "Fuzhou", pinyin: "fuzhou", py: "fz", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
@@ -5807,12 +5900,15 @@
         <v>137</v>
       </c>
       <c r="H30" s="1"/>
-      <c r="J30" s="2" t="str">
+      <c r="I30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "hf", lat: 31.798265, lng: 117.29036, name: "合肥", english: "Hefei", pinyin: "hefei", py: "hf", other: "" },</v>
+        <v>{ key: "hf", lat: 31.798265, lng: 117.29036, name: "合肥", english: "Hefei", pinyin: "hefei", py: "hf", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>64</v>
       </c>
@@ -5835,12 +5931,15 @@
         <v>138</v>
       </c>
       <c r="H31" s="1"/>
-      <c r="J31" s="2" t="str">
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+      <c r="K31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "sj", lat: 38.043229, lng: 114.477312, name: "石家庄", english: "Shijiazhuang", pinyin: "shijiazhuang", py: "sjz", other: "" },</v>
+        <v>{ key: "sj", lat: 38.043229, lng: 114.477312, name: "石家庄", english: "Shijiazhuang", pinyin: "shijiazhuang", py: "sjz", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>65</v>
       </c>
@@ -5863,12 +5962,15 @@
         <v>139</v>
       </c>
       <c r="H32" s="1"/>
-      <c r="J32" s="2" t="str">
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "xm", lat: 24.602695, lng: 118.054655, name: "厦门", english: "Xiamen", pinyin: "xiamen", py: "xm", other: "" },</v>
+        <v>{ key: "xm", lat: 24.602695, lng: 118.054655, name: "厦门", english: "Xiamen", pinyin: "xiamen", py: "xm", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>66</v>
       </c>
@@ -5891,12 +5993,15 @@
         <v>140</v>
       </c>
       <c r="H33" s="1"/>
-      <c r="J33" s="2" t="str">
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "gy", lat: 26.619416, lng: 106.675967, name: "贵阳", english: "Guiyang", pinyin: "guiyang", py: "gy", other: "" },</v>
+        <v>{ key: "gy", lat: 26.619416, lng: 106.675967, name: "贵阳", english: "Guiyang", pinyin: "guiyang", py: "gy", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>67</v>
       </c>
@@ -5919,12 +6024,15 @@
         <v>141</v>
       </c>
       <c r="H34" s="1"/>
-      <c r="J34" s="2" t="str">
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+      <c r="K34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "gx", lat: 22.631423, lng: 120.30195, name: "高雄", english: "Kaohsiung", pinyin: "gaoxiong", py: "gx", other: "" },</v>
+        <v>{ key: "gx", lat: 22.631423, lng: 120.30195, name: "高雄", english: "Kaohsiung", pinyin: "gaoxiong", py: "gx", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
@@ -5949,12 +6057,15 @@
       <c r="H35" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="J35" s="2" t="str">
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+      <c r="K35" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "wl", lat: 43.840204, lng: 87.574904, name: "乌鲁木齐", english: "Urumqi", pinyin: "wulumuqi", py: "wlmq", other: "urmq|urumqi" },</v>
+        <v>{ key: "wl", lat: 43.840204, lng: 87.574904, name: "乌鲁木齐", english: "Urumqi", pinyin: "wulumuqi", py: "wlmq", other: "urmq|urumqi", plan: "0" },</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>69</v>
       </c>
@@ -5977,12 +6088,15 @@
         <v>145</v>
       </c>
       <c r="H36" s="1"/>
-      <c r="J36" s="2" t="str">
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "wz", lat: 27.979144, lng: 120.68513, name: "温州", english: "Wenzhou", pinyin: "wenzhou", py: "wz", other: "" },</v>
+        <v>{ key: "wz", lat: 27.979144, lng: 120.68513, name: "温州", english: "Wenzhou", pinyin: "wenzhou", py: "wz", other: "", plan: "0" },</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>516</v>
       </c>
@@ -6005,9 +6119,12 @@
         <v>515</v>
       </c>
       <c r="H37" s="1"/>
-      <c r="J37" s="2" t="str">
+      <c r="I37" s="1">
+        <v>0</v>
+      </c>
+      <c r="K37" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "jn", lat: 36.669337, lng: 116.893471, name: "济南", english: "Jinan", pinyin: "jinan", py: "jn", other: "" },</v>
+        <v>{ key: "jn", lat: 36.669337, lng: 116.893471, name: "济南", english: "Jinan", pinyin: "jinan", py: "jn", other: "", plan: "0" },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support metro plan map
</commit_message>
<xml_diff>
--- a/doc/data.xlsx
+++ b/doc/data.xlsx
@@ -597,32 +597,6 @@
   </si>
   <si>
     <r>
-      <t>T3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t>航站楼</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>T2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t>航站楼</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="9"/>
         <color theme="1"/>
@@ -4564,6 +4538,42 @@
   </si>
   <si>
     <t>Plan</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>号航站楼</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>号</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>航站楼</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4955,7 +4965,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K37" sqref="K2:K37"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -4997,7 +5007,7 @@
         <v>106</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>146</v>
@@ -5014,7 +5024,7 @@
         <v>116.411502</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
@@ -5045,7 +5055,7 @@
         <v>121.47537</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>2</v>
@@ -5076,7 +5086,7 @@
         <v>113.32410299999999</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>3</v>
@@ -5091,11 +5101,11 @@
         <v>161</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "gz", lat: 23.111459, lng: 113.324103, name: "广州(佛山)", english: "Guangzhou", pinyin: "guangzhou", py: "gz", other: "foshan|fs", plan: "0" },</v>
+        <v>{ key: "gz", lat: 23.111459, lng: 113.324103, name: "广州(佛山)", english: "Guangzhou", pinyin: "guangzhou", py: "gz", other: "foshan|fs", plan: "1" },</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
@@ -5109,7 +5119,7 @@
         <v>114.05282699999999</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
@@ -5140,7 +5150,7 @@
         <v>114.158185</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
@@ -5155,11 +5165,11 @@
         <v>147</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "hk", lat: 22.284659, lng: 114.158185, name: "香港", english: "Hong Kong", pinyin: "xianggang", py: "xg", other: "hk|hongkong|hong kong", plan: "0" },</v>
+        <v>{ key: "hk", lat: 22.284659, lng: 114.158185, name: "香港", english: "Hong Kong", pinyin: "xianggang", py: "xg", other: "hk|hongkong|hong kong", plan: "1" },</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
@@ -5173,7 +5183,7 @@
         <v>121.51752999999999</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>6</v>
@@ -5206,7 +5216,7 @@
         <v>118.78408</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>7</v>
@@ -5237,7 +5247,7 @@
         <v>117.21160999999999</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
@@ -5268,7 +5278,7 @@
         <v>106.54827299999999</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>9</v>
@@ -5299,7 +5309,7 @@
         <v>104.065798</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>10</v>
@@ -5330,7 +5340,7 @@
         <v>114.286584</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>11</v>
@@ -5361,7 +5371,7 @@
         <v>120.165666</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
@@ -5374,11 +5384,11 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "hz", lat: 30.279156, lng: 120.165666, name: "杭州", english: "Hangzhou", pinyin: "hangzhou", py: "hz", other: "", plan: "0" },</v>
+        <v>{ key: "hz", lat: 30.279156, lng: 120.165666, name: "杭州", english: "Hangzhou", pinyin: "hangzhou", py: "hz", other: "", plan: "1" },</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
@@ -5392,7 +5402,7 @@
         <v>108.947143</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>13</v>
@@ -5423,7 +5433,7 @@
         <v>120.54929199999999</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>14</v>
@@ -5454,7 +5464,7 @@
         <v>123.433386</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>15</v>
@@ -5485,7 +5495,7 @@
         <v>125.365183</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>16</v>
@@ -5516,7 +5526,7 @@
         <v>126.643805</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>17</v>
@@ -5547,7 +5557,7 @@
         <v>112.97635699999999</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>18</v>
@@ -5578,7 +5588,7 @@
         <v>121.548731</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>19</v>
@@ -5609,7 +5619,7 @@
         <v>120.306895</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>20</v>
@@ -5640,7 +5650,7 @@
         <v>113.655446</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>21</v>
@@ -5671,7 +5681,7 @@
         <v>121.587378</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>22</v>
@@ -5702,7 +5712,7 @@
         <v>102.72384700000001</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>23</v>
@@ -5733,7 +5743,7 @@
         <v>115.903436</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>24</v>
@@ -5764,7 +5774,7 @@
         <v>120.376824</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>25</v>
@@ -5777,11 +5787,11 @@
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "qd", lat: 36.169772, lng: 120.376824, name: "青岛", english: "Qingdao", pinyin: "qingdao", py: "qd", other: "", plan: "0" },</v>
+        <v>{ key: "qd", lat: 36.169772, lng: 120.376824, name: "青岛", english: "Qingdao", pinyin: "qingdao", py: "qd", other: "", plan: "1" },</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.15">
@@ -5795,7 +5805,7 @@
         <v>113.860969</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>26</v>
@@ -5826,7 +5836,7 @@
         <v>108.413459</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>27</v>
@@ -5857,7 +5867,7 @@
         <v>119.39006000000001</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>28</v>
@@ -5888,7 +5898,7 @@
         <v>117.29036000000001</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>29</v>
@@ -5919,7 +5929,7 @@
         <v>114.477312</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>30</v>
@@ -5950,7 +5960,7 @@
         <v>118.054655</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>31</v>
@@ -5981,7 +5991,7 @@
         <v>106.675967</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>32</v>
@@ -6012,7 +6022,7 @@
         <v>120.30195000000001</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>33</v>
@@ -6043,7 +6053,7 @@
         <v>87.574904000000004</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>34</v>
@@ -6058,11 +6068,11 @@
         <v>149</v>
       </c>
       <c r="I35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "wl", lat: 43.840204, lng: 87.574904, name: "乌鲁木齐", english: "Urumqi", pinyin: "wulumuqi", py: "wlmq", other: "urmq|urumqi", plan: "0" },</v>
+        <v>{ key: "wl", lat: 43.840204, lng: 87.574904, name: "乌鲁木齐", english: "Urumqi", pinyin: "wulumuqi", py: "wlmq", other: "urmq|urumqi", plan: "1" },</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.15">
@@ -6076,7 +6086,7 @@
         <v>120.68513</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>35</v>
@@ -6089,16 +6099,16 @@
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "wz", lat: 27.979144, lng: 120.68513, name: "温州", english: "Wenzhou", pinyin: "wenzhou", py: "wz", other: "", plan: "0" },</v>
+        <v>{ key: "wz", lat: 27.979144, lng: 120.68513, name: "温州", english: "Wenzhou", pinyin: "wenzhou", py: "wz", other: "", plan: "1" },</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B37" s="1">
         <v>36.669336999999999</v>
@@ -6107,24 +6117,24 @@
         <v>116.89347100000001</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ key: "jn", lat: 36.669337, lng: 116.893471, name: "济南", english: "Jinan", pinyin: "jinan", py: "jn", other: "", plan: "0" },</v>
+        <v>{ key: "jn", lat: 36.669337, lng: 116.893471, name: "济南", english: "Jinan", pinyin: "jinan", py: "jn", other: "", plan: "1" },</v>
       </c>
     </row>
   </sheetData>
@@ -6138,7 +6148,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
@@ -6211,29 +6223,29 @@
         <v>165</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="N2" s="2" t="str">
         <f>"{ key: """ &amp; A2 &amp; """, hot: [" &amp; """" &amp; C2 &amp; """" &amp; IF(D2 = "", "", ", """ &amp; D2 &amp; """") &amp; IF(E2 = "", "", ", """ &amp; E2 &amp; """") &amp; IF(F2 = "", "", ", """ &amp; F2 &amp; """") &amp; IF(G2 = "", "", ", """ &amp; G2 &amp; """") &amp; IF(H2 = "", "", ", """ &amp; H2 &amp; """") &amp; IF(I2 = "", "", ", """ &amp; I2 &amp; """") &amp; IF(J2 = "", "", ", """ &amp; J2 &amp; """") &amp; IF(K2 = "", "", ", """ &amp; K2 &amp; """") &amp; IF(L2 = "", "", ", """ &amp; L2 &amp; """") &amp; "] },"</f>
-        <v>{ key: "bj", hot: ["北京南站", "北京西站", "北京站", "T3航站楼", "T2航站楼", "东直门", "西直门", "天安门东", "前门", "国贸"] },</v>
+        <v>{ key: "bj", hot: ["北京南站", "北京西站", "北京站", "3号航站楼", "2号航站楼", "东直门", "西直门", "天安门东", "前门", "国贸"] },</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
@@ -6241,37 +6253,37 @@
         <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="N3" s="2" t="str">
         <f t="shared" ref="N3:N37" si="0">"{ key: """ &amp; A3 &amp; """, hot: [" &amp; """" &amp; C3 &amp; """" &amp; IF(D3 = "", "", ", """ &amp; D3 &amp; """") &amp; IF(E3 = "", "", ", """ &amp; E3 &amp; """") &amp; IF(F3 = "", "", ", """ &amp; F3 &amp; """") &amp; IF(G3 = "", "", ", """ &amp; G3 &amp; """") &amp; IF(H3 = "", "", ", """ &amp; H3 &amp; """") &amp; IF(I3 = "", "", ", """ &amp; I3 &amp; """") &amp; IF(J3 = "", "", ", """ &amp; J3 &amp; """") &amp; IF(K3 = "", "", ", """ &amp; K3 &amp; """") &amp; IF(L3 = "", "", ", """ &amp; L3 &amp; """") &amp; "] },"</f>
@@ -6283,37 +6295,37 @@
         <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="N4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6325,37 +6337,37 @@
         <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="N5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6367,37 +6379,37 @@
         <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="H6" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="N6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6409,37 +6421,37 @@
         <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="N7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6451,37 +6463,37 @@
         <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="N8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6493,37 +6505,37 @@
         <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="K9" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="N9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6535,37 +6547,37 @@
         <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="N10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6577,37 +6589,37 @@
         <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="N11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6619,37 +6631,37 @@
         <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="I12" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="N12" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6661,37 +6673,37 @@
         <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="N13" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6703,37 +6715,37 @@
         <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="N14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6745,37 +6757,37 @@
         <v>48</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>311</v>
       </c>
       <c r="N15" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6787,37 +6799,37 @@
         <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>322</v>
       </c>
       <c r="N16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6829,37 +6841,37 @@
         <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="F17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>331</v>
-      </c>
       <c r="L17" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="N17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6871,37 +6883,37 @@
         <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>340</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>342</v>
       </c>
       <c r="N18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6913,37 +6925,37 @@
         <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="E19" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>352</v>
       </c>
       <c r="N19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6955,37 +6967,37 @@
         <v>53</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="E20" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>361</v>
       </c>
       <c r="N20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -6997,37 +7009,37 @@
         <v>54</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="I21" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="J21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="N21" s="2" t="str">
         <f t="shared" si="0"/>
@@ -7039,37 +7051,37 @@
         <v>55</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="H22" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="I22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>381</v>
       </c>
       <c r="N22" s="2" t="str">
         <f t="shared" si="0"/>
@@ -7081,37 +7093,37 @@
         <v>56</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="E23" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="J23" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>390</v>
       </c>
       <c r="N23" s="2" t="str">
         <f t="shared" si="0"/>
@@ -7123,37 +7135,37 @@
         <v>57</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>399</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>401</v>
       </c>
       <c r="N24" s="2" t="str">
         <f t="shared" si="0"/>
@@ -7165,37 +7177,37 @@
         <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>411</v>
-      </c>
       <c r="L25" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="N25" s="2" t="str">
         <f t="shared" si="0"/>
@@ -7207,37 +7219,37 @@
         <v>59</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="H26" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="J26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>418</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="N26" s="2" t="str">
         <f t="shared" si="0"/>
@@ -7249,28 +7261,28 @@
         <v>60</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>428</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -7285,37 +7297,37 @@
         <v>61</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="K28" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="L28" s="1" t="s">
         <v>436</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>438</v>
       </c>
       <c r="N28" s="2" t="str">
         <f t="shared" si="0"/>
@@ -7327,22 +7339,22 @@
         <v>62</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>442</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>444</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -7359,34 +7371,34 @@
         <v>63</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>454</v>
       </c>
       <c r="L30" s="1"/>
       <c r="N30" s="2" t="str">
@@ -7399,37 +7411,37 @@
         <v>64</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>463</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>465</v>
       </c>
       <c r="N31" s="2" t="str">
         <f t="shared" si="0"/>
@@ -7441,34 +7453,34 @@
         <v>65</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="F32" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="G32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>472</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>474</v>
       </c>
       <c r="L32" s="1"/>
       <c r="N32" s="2" t="str">
@@ -7481,28 +7493,28 @@
         <v>66</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>480</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>482</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -7517,37 +7529,37 @@
         <v>67</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>493</v>
       </c>
       <c r="N34" s="2" t="str">
         <f t="shared" si="0"/>
@@ -7559,22 +7571,22 @@
         <v>68</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>497</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -7591,34 +7603,34 @@
         <v>69</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="E36" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>506</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>508</v>
       </c>
       <c r="L36" s="1"/>
       <c r="N36" s="2" t="str">
@@ -7628,28 +7640,28 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="E37" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="F37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>512</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>514</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>

</xml_diff>